<commit_message>
updated schema in excel file
</commit_message>
<xml_diff>
--- a/Database/DatabaseSchema.xlsx
+++ b/Database/DatabaseSchema.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25600" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Doctors</t>
   </si>
@@ -60,9 +60,6 @@
     <t>statUpperBound</t>
   </si>
   <si>
-    <t>recipientPhoneNumber</t>
-  </si>
-  <si>
     <t>callsOn</t>
   </si>
   <si>
@@ -75,20 +72,32 @@
     <t>patientName</t>
   </si>
   <si>
-    <t>recipientName</t>
-  </si>
-  <si>
     <t>doctorPhoneNumber</t>
   </si>
   <si>
     <t>doctorAddress</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>contact_id</t>
+  </si>
+  <si>
+    <t>contactName</t>
+  </si>
+  <si>
+    <t>contactPhoneNumber</t>
+  </si>
+  <si>
+    <t>Patients_Contacts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,6 +120,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -129,15 +154,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -478,7 +536,7 @@
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -492,13 +550,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1"/>
       <c r="J2" t="s">
@@ -528,6 +586,17 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="J6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
@@ -539,7 +608,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -563,28 +632,45 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E17" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>